<commit_message>
Cambio descripción pequeña plantilla auditoria
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.4 Plantilla_Auditoria_energetica.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.4 Plantilla_Auditoria_energetica.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Web Dinamico 2\MRVMinem\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B67AB-2546-4077-AD53-AAE72D7B1583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A750A9-C10F-420E-A582-924FBF19B2DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2E5039C4-2A71-47B3-941E-557D52B97803}"/>
   </bookViews>
@@ -231,9 +231,6 @@
     <t>Fuente de energía utilizada para el funcionamiento de el/los equipos y/o desarrollo del proceso. Seleccione de la lista desplegable.</t>
   </si>
   <si>
-    <t>Total del consumo del energético para el funcionamiento del/los equipos y/o desarrollo del proceso durante un año. Inserte sus datos.</t>
-  </si>
-  <si>
     <t>Unidad de medición del energético. Seleccione de la lista desplegable.</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>Cantidad de equipos a mejorar o cambiar por recomendación de la auditoría. En caso de mejora de proceso, colocar 1. Ingrese sus datos.</t>
-  </si>
-  <si>
-    <t>Total de unidades del energético durante un año para el funcionamiento de el/los equipos y/o desarrollo del proceso. Ingrese sus datos.</t>
   </si>
   <si>
     <t>Unidad de medición. Seleccione de la lista desplegable.</t>
@@ -293,6 +287,108 @@
   <si>
     <t>Estado</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Total del consumo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">energético </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unitario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para el funcionamiento del equipo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y/o desarrollo del proceso. Ingrese sus datos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total del </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>consumo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> energético </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unitario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para el funcionamiento del equipo y/o desarrollo del proceso durante un año. Inserte sus datos.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +445,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -993,27 +1096,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,6 +1150,27 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFC1772-35AF-4198-9510-18D55384E446}">
   <dimension ref="A1:AE317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,43 +1526,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="110" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="52"/>
-      <c r="C1" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="92" t="s">
+      <c r="C1" s="111" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="O1" s="114" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="AC1" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="O1" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="AC1" s="95" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD1" s="95"/>
-      <c r="AE1" s="95"/>
+      <c r="AD1" s="115"/>
+      <c r="AE1" s="115"/>
     </row>
     <row r="2" spans="1:31" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
+      <c r="A2" s="110"/>
       <c r="B2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="91"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="84" t="s">
         <v>12</v>
       </c>
@@ -1470,10 +1573,10 @@
         <v>4</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I2" s="54" t="s">
         <v>4</v>
@@ -1516,49 +1619,49 @@
         <v>10</v>
       </c>
       <c r="AC2" s="56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AD2" s="57" t="s">
         <v>53</v>
       </c>
       <c r="AE2" s="56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="89"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109"/>
     </row>
     <row r="4" spans="1:31" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
@@ -1579,32 +1682,32 @@
         <v>62</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
       <c r="M4" s="49"/>
       <c r="N4" s="49"/>
       <c r="O4" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="49" t="s">
         <v>65</v>
-      </c>
-      <c r="P4" s="49" t="s">
-        <v>66</v>
       </c>
       <c r="Q4" s="49"/>
       <c r="R4" s="49" t="s">
         <v>62</v>
       </c>
       <c r="S4" s="49" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="T4" s="49"/>
       <c r="U4" s="50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -1614,13 +1717,13 @@
       <c r="AA4" s="49"/>
       <c r="AB4" s="67"/>
       <c r="AC4" s="68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AD4" s="51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AE4" s="49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="75" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AD5" s="76">
         <v>7306</v>
@@ -24693,57 +24796,57 @@
         <f t="shared" si="27"/>
         <v>#N/A</v>
       </c>
-      <c r="J312" s="96"/>
-      <c r="K312" s="97">
-        <v>0</v>
-      </c>
-      <c r="L312" s="97">
-        <v>0</v>
-      </c>
-      <c r="M312" s="97">
-        <v>0</v>
-      </c>
-      <c r="N312" s="97">
-        <v>0</v>
-      </c>
-      <c r="O312" s="98"/>
-      <c r="P312" s="99"/>
-      <c r="Q312" s="100" t="e">
+      <c r="J312" s="89"/>
+      <c r="K312" s="90">
+        <v>0</v>
+      </c>
+      <c r="L312" s="90">
+        <v>0</v>
+      </c>
+      <c r="M312" s="90">
+        <v>0</v>
+      </c>
+      <c r="N312" s="90">
+        <v>0</v>
+      </c>
+      <c r="O312" s="91"/>
+      <c r="P312" s="92"/>
+      <c r="Q312" s="93" t="e">
         <f t="shared" si="28"/>
         <v>#N/A</v>
       </c>
-      <c r="R312" s="101"/>
-      <c r="S312" s="102"/>
-      <c r="T312" s="103" t="e">
+      <c r="R312" s="94"/>
+      <c r="S312" s="95"/>
+      <c r="T312" s="96" t="e">
         <f t="shared" si="29"/>
         <v>#N/A</v>
       </c>
-      <c r="U312" s="104"/>
-      <c r="V312" s="105">
-        <v>0</v>
-      </c>
-      <c r="W312" s="105">
-        <v>0</v>
-      </c>
-      <c r="X312" s="105">
-        <v>0</v>
-      </c>
-      <c r="Y312" s="105">
-        <v>0</v>
-      </c>
-      <c r="Z312" s="105">
-        <v>0</v>
-      </c>
-      <c r="AA312" s="105">
-        <v>0</v>
-      </c>
-      <c r="AB312" s="106" t="e">
+      <c r="U312" s="97"/>
+      <c r="V312" s="98">
+        <v>0</v>
+      </c>
+      <c r="W312" s="98">
+        <v>0</v>
+      </c>
+      <c r="X312" s="98">
+        <v>0</v>
+      </c>
+      <c r="Y312" s="98">
+        <v>0</v>
+      </c>
+      <c r="Z312" s="98">
+        <v>0</v>
+      </c>
+      <c r="AA312" s="98">
+        <v>0</v>
+      </c>
+      <c r="AB312" s="99" t="e">
         <f t="shared" si="30"/>
         <v>#N/A</v>
       </c>
-      <c r="AC312" s="107"/>
-      <c r="AD312" s="108"/>
-      <c r="AE312" s="108"/>
+      <c r="AC312" s="100"/>
+      <c r="AD312" s="101"/>
+      <c r="AE312" s="101"/>
     </row>
     <row r="313" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A313" s="26"/>
@@ -24764,28 +24867,28 @@
         <f t="shared" si="27"/>
         <v>#N/A</v>
       </c>
-      <c r="J313" s="96"/>
-      <c r="K313" s="109"/>
-      <c r="L313" s="109"/>
-      <c r="M313" s="109"/>
-      <c r="N313" s="109"/>
-      <c r="O313" s="98"/>
-      <c r="P313" s="99"/>
-      <c r="Q313" s="110"/>
-      <c r="R313" s="110"/>
-      <c r="S313" s="110"/>
-      <c r="T313" s="110"/>
-      <c r="U313" s="110"/>
-      <c r="V313" s="110"/>
-      <c r="W313" s="110"/>
-      <c r="X313" s="110"/>
-      <c r="Y313" s="110"/>
-      <c r="Z313" s="110"/>
-      <c r="AA313" s="110"/>
-      <c r="AB313" s="110"/>
-      <c r="AC313" s="110"/>
-      <c r="AD313" s="108"/>
-      <c r="AE313" s="108"/>
+      <c r="J313" s="89"/>
+      <c r="K313" s="102"/>
+      <c r="L313" s="102"/>
+      <c r="M313" s="102"/>
+      <c r="N313" s="102"/>
+      <c r="O313" s="91"/>
+      <c r="P313" s="92"/>
+      <c r="Q313" s="103"/>
+      <c r="R313" s="103"/>
+      <c r="S313" s="103"/>
+      <c r="T313" s="103"/>
+      <c r="U313" s="103"/>
+      <c r="V313" s="103"/>
+      <c r="W313" s="103"/>
+      <c r="X313" s="103"/>
+      <c r="Y313" s="103"/>
+      <c r="Z313" s="103"/>
+      <c r="AA313" s="103"/>
+      <c r="AB313" s="103"/>
+      <c r="AC313" s="103"/>
+      <c r="AD313" s="101"/>
+      <c r="AE313" s="101"/>
     </row>
     <row r="314" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A314" s="33"/>
@@ -24797,28 +24900,28 @@
       <c r="G314" s="33"/>
       <c r="H314" s="33"/>
       <c r="I314" s="33"/>
-      <c r="J314" s="110"/>
-      <c r="K314" s="110"/>
-      <c r="L314" s="110"/>
-      <c r="M314" s="110"/>
-      <c r="N314" s="110"/>
-      <c r="O314" s="98"/>
-      <c r="P314" s="99"/>
-      <c r="Q314" s="110"/>
-      <c r="R314" s="110"/>
-      <c r="S314" s="110"/>
-      <c r="T314" s="110"/>
-      <c r="U314" s="110"/>
-      <c r="V314" s="110"/>
-      <c r="W314" s="110"/>
-      <c r="X314" s="110"/>
-      <c r="Y314" s="110"/>
-      <c r="Z314" s="110"/>
-      <c r="AA314" s="110"/>
-      <c r="AB314" s="110"/>
-      <c r="AC314" s="110"/>
-      <c r="AD314" s="111"/>
-      <c r="AE314" s="108"/>
+      <c r="J314" s="103"/>
+      <c r="K314" s="103"/>
+      <c r="L314" s="103"/>
+      <c r="M314" s="103"/>
+      <c r="N314" s="103"/>
+      <c r="O314" s="91"/>
+      <c r="P314" s="92"/>
+      <c r="Q314" s="103"/>
+      <c r="R314" s="103"/>
+      <c r="S314" s="103"/>
+      <c r="T314" s="103"/>
+      <c r="U314" s="103"/>
+      <c r="V314" s="103"/>
+      <c r="W314" s="103"/>
+      <c r="X314" s="103"/>
+      <c r="Y314" s="103"/>
+      <c r="Z314" s="103"/>
+      <c r="AA314" s="103"/>
+      <c r="AB314" s="103"/>
+      <c r="AC314" s="103"/>
+      <c r="AD314" s="104"/>
+      <c r="AE314" s="101"/>
     </row>
     <row r="315" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A315" s="19"/>
@@ -24830,28 +24933,28 @@
       <c r="G315" s="19"/>
       <c r="H315" s="19"/>
       <c r="I315" s="19"/>
-      <c r="J315" s="112"/>
-      <c r="K315" s="112"/>
-      <c r="L315" s="112"/>
-      <c r="M315" s="112"/>
-      <c r="N315" s="112"/>
-      <c r="O315" s="113"/>
-      <c r="P315" s="114"/>
-      <c r="Q315" s="112"/>
-      <c r="R315" s="112"/>
-      <c r="S315" s="112"/>
-      <c r="T315" s="112"/>
-      <c r="U315" s="112"/>
-      <c r="V315" s="112"/>
-      <c r="W315" s="112"/>
-      <c r="X315" s="112"/>
-      <c r="Y315" s="112"/>
-      <c r="Z315" s="112"/>
-      <c r="AA315" s="112"/>
-      <c r="AB315" s="112"/>
-      <c r="AC315" s="112"/>
-      <c r="AD315" s="115"/>
-      <c r="AE315" s="112"/>
+      <c r="J315" s="105"/>
+      <c r="K315" s="105"/>
+      <c r="L315" s="105"/>
+      <c r="M315" s="105"/>
+      <c r="N315" s="105"/>
+      <c r="O315" s="106"/>
+      <c r="P315" s="107"/>
+      <c r="Q315" s="105"/>
+      <c r="R315" s="105"/>
+      <c r="S315" s="105"/>
+      <c r="T315" s="105"/>
+      <c r="U315" s="105"/>
+      <c r="V315" s="105"/>
+      <c r="W315" s="105"/>
+      <c r="X315" s="105"/>
+      <c r="Y315" s="105"/>
+      <c r="Z315" s="105"/>
+      <c r="AA315" s="105"/>
+      <c r="AB315" s="105"/>
+      <c r="AC315" s="105"/>
+      <c r="AD315" s="108"/>
+      <c r="AE315" s="105"/>
     </row>
     <row r="316" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A316" s="19"/>
@@ -24863,55 +24966,55 @@
       <c r="G316" s="19"/>
       <c r="H316" s="19"/>
       <c r="I316" s="19"/>
-      <c r="J316" s="112"/>
-      <c r="K316" s="112"/>
-      <c r="L316" s="112"/>
-      <c r="M316" s="112"/>
-      <c r="N316" s="112"/>
-      <c r="O316" s="113"/>
-      <c r="P316" s="112"/>
-      <c r="Q316" s="112"/>
-      <c r="R316" s="112"/>
-      <c r="S316" s="112"/>
-      <c r="T316" s="112"/>
-      <c r="U316" s="112"/>
-      <c r="V316" s="112"/>
-      <c r="W316" s="112"/>
-      <c r="X316" s="112"/>
-      <c r="Y316" s="112"/>
-      <c r="Z316" s="112"/>
-      <c r="AA316" s="112"/>
-      <c r="AB316" s="112"/>
-      <c r="AC316" s="112"/>
-      <c r="AD316" s="115"/>
-      <c r="AE316" s="112"/>
+      <c r="J316" s="105"/>
+      <c r="K316" s="105"/>
+      <c r="L316" s="105"/>
+      <c r="M316" s="105"/>
+      <c r="N316" s="105"/>
+      <c r="O316" s="106"/>
+      <c r="P316" s="105"/>
+      <c r="Q316" s="105"/>
+      <c r="R316" s="105"/>
+      <c r="S316" s="105"/>
+      <c r="T316" s="105"/>
+      <c r="U316" s="105"/>
+      <c r="V316" s="105"/>
+      <c r="W316" s="105"/>
+      <c r="X316" s="105"/>
+      <c r="Y316" s="105"/>
+      <c r="Z316" s="105"/>
+      <c r="AA316" s="105"/>
+      <c r="AB316" s="105"/>
+      <c r="AC316" s="105"/>
+      <c r="AD316" s="108"/>
+      <c r="AE316" s="105"/>
     </row>
     <row r="317" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="J317" s="112"/>
-      <c r="K317" s="112"/>
-      <c r="L317" s="112"/>
-      <c r="M317" s="112"/>
-      <c r="N317" s="112"/>
-      <c r="O317" s="113"/>
-      <c r="P317" s="112"/>
-      <c r="Q317" s="112"/>
-      <c r="R317" s="112"/>
-      <c r="S317" s="112"/>
-      <c r="T317" s="112"/>
-      <c r="U317" s="112"/>
-      <c r="V317" s="112"/>
-      <c r="W317" s="112"/>
-      <c r="X317" s="112"/>
-      <c r="Y317" s="112"/>
-      <c r="Z317" s="112"/>
-      <c r="AA317" s="112"/>
-      <c r="AB317" s="112"/>
-      <c r="AC317" s="112"/>
-      <c r="AD317" s="112"/>
-      <c r="AE317" s="112"/>
+      <c r="J317" s="105"/>
+      <c r="K317" s="105"/>
+      <c r="L317" s="105"/>
+      <c r="M317" s="105"/>
+      <c r="N317" s="105"/>
+      <c r="O317" s="106"/>
+      <c r="P317" s="105"/>
+      <c r="Q317" s="105"/>
+      <c r="R317" s="105"/>
+      <c r="S317" s="105"/>
+      <c r="T317" s="105"/>
+      <c r="U317" s="105"/>
+      <c r="V317" s="105"/>
+      <c r="W317" s="105"/>
+      <c r="X317" s="105"/>
+      <c r="Y317" s="105"/>
+      <c r="Z317" s="105"/>
+      <c r="AA317" s="105"/>
+      <c r="AB317" s="105"/>
+      <c r="AC317" s="105"/>
+      <c r="AD317" s="105"/>
+      <c r="AE317" s="105"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+X+Rs9jU+9ODySX4ttO+9ZXjzG3QyhJhYcaysox7MCvzbnNBB2+I6WM2b8hvFb/78dOIu7htTJuWtTcSz0Ryxw==" saltValue="1gcmNpRLFa/7DiI/iS64BA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sWc8uI7kgkNNjX9+d4X5ctt2yrs4SJ7SqHptsS3c4PpOEEVbkyYYx+z4NwhuvKF4FHuVOKtZ0SASFtza4NW2AQ==" saltValue="ZIiw83ilTB6o+rhwT7b3vA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="A3:AE3"/>
     <mergeCell ref="A1:A2"/>
@@ -25006,7 +25109,7 @@
         <v>8</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U4" s="12" t="s">
         <v>8</v>
@@ -25041,7 +25144,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R5" s="11">
         <v>1</v>
@@ -25082,7 +25185,7 @@
         <v>2</v>
       </c>
       <c r="Q6" s="47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R6" s="47">
         <v>2</v>
@@ -25123,7 +25226,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R7" s="4">
         <v>3</v>

</xml_diff>